<commit_message>
Documentação completa da Sprint 6
</commit_message>
<xml_diff>
--- a/Sprint 6/Product Backlog-Burndown.xlsx
+++ b/Sprint 6/Product Backlog-Burndown.xlsx
@@ -807,11 +807,41 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -831,59 +861,29 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1124,7 +1124,7 @@
               <c15:filteredCategoryTitle>
                 <c15:cat>
                   <c:strRef>
-                    <c:extLst xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart">
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>categories</c15:sqref>
@@ -1242,19 +1242,19 @@
                   <c:v>356.16999999999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>342.91999999999996</c:v>
+                  <c:v>318.46999999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>342.91999999999996</c:v>
+                  <c:v>318.46999999999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>342.91999999999996</c:v>
+                  <c:v>318.46999999999997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>342.91999999999996</c:v>
+                  <c:v>318.46999999999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>342.91999999999996</c:v>
+                  <c:v>318.46999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1268,7 +1268,7 @@
               <c15:filteredCategoryTitle>
                 <c15:cat>
                   <c:strRef>
-                    <c:extLst xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart">
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>categories</c15:sqref>
@@ -1334,11 +1334,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="229242256"/>
-        <c:axId val="219880632"/>
+        <c:axId val="226281528"/>
+        <c:axId val="226282312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="229242256"/>
+        <c:axId val="226281528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1373,7 +1373,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="219880632"/>
+        <c:crossAx val="226282312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1381,7 +1381,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="219880632"/>
+        <c:axId val="226282312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="500"/>
@@ -1427,7 +1427,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="229242256"/>
+        <c:crossAx val="226281528"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1811,8 +1811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S65"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1827,14 +1827,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -2038,10 +2038,10 @@
       <c r="S7" s="1"/>
     </row>
     <row r="8" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="61" t="s">
+      <c r="A8" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="62" t="s">
+      <c r="B8" s="54" t="s">
         <v>41</v>
       </c>
       <c r="C8" s="22" t="s">
@@ -2071,8 +2071,8 @@
       <c r="S8" s="1"/>
     </row>
     <row r="9" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="61"/>
-      <c r="B9" s="63"/>
+      <c r="A9" s="53"/>
+      <c r="B9" s="55"/>
       <c r="C9" s="23" t="s">
         <v>43</v>
       </c>
@@ -2100,8 +2100,8 @@
       <c r="S9" s="1"/>
     </row>
     <row r="10" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="61"/>
-      <c r="B10" s="63"/>
+      <c r="A10" s="53"/>
+      <c r="B10" s="55"/>
       <c r="C10" s="23" t="s">
         <v>44</v>
       </c>
@@ -2129,8 +2129,8 @@
       <c r="S10" s="1"/>
     </row>
     <row r="11" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="61"/>
-      <c r="B11" s="63"/>
+      <c r="A11" s="53"/>
+      <c r="B11" s="55"/>
       <c r="C11" s="23" t="s">
         <v>45</v>
       </c>
@@ -2158,8 +2158,8 @@
       <c r="S11" s="1"/>
     </row>
     <row r="12" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="61"/>
-      <c r="B12" s="63"/>
+      <c r="A12" s="53"/>
+      <c r="B12" s="55"/>
       <c r="C12" s="23" t="s">
         <v>46</v>
       </c>
@@ -2187,8 +2187,8 @@
       <c r="S12" s="1"/>
     </row>
     <row r="13" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="61"/>
-      <c r="B13" s="63"/>
+      <c r="A13" s="53"/>
+      <c r="B13" s="55"/>
       <c r="C13" s="23" t="s">
         <v>47</v>
       </c>
@@ -2216,8 +2216,8 @@
       <c r="S13" s="1"/>
     </row>
     <row r="14" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="61"/>
-      <c r="B14" s="64"/>
+      <c r="A14" s="53"/>
+      <c r="B14" s="56"/>
       <c r="C14" s="23" t="s">
         <v>48</v>
       </c>
@@ -2245,7 +2245,7 @@
       <c r="S14" s="1"/>
     </row>
     <row r="15" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A15" s="55" t="s">
+      <c r="A15" s="49" t="s">
         <v>49</v>
       </c>
       <c r="B15" s="46" t="s">
@@ -2278,8 +2278,8 @@
       <c r="S15" s="1"/>
     </row>
     <row r="16" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A16" s="59"/>
-      <c r="B16" s="47"/>
+      <c r="A16" s="50"/>
+      <c r="B16" s="48"/>
       <c r="C16" s="24" t="s">
         <v>52</v>
       </c>
@@ -2307,8 +2307,8 @@
       <c r="S16" s="1"/>
     </row>
     <row r="17" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="59"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="50"/>
+      <c r="B17" s="48"/>
       <c r="C17" s="24" t="s">
         <v>54</v>
       </c>
@@ -2336,8 +2336,8 @@
       <c r="S17" s="1"/>
     </row>
     <row r="18" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="56"/>
-      <c r="B18" s="48"/>
+      <c r="A18" s="51"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="25" t="s">
         <v>53</v>
       </c>
@@ -2365,7 +2365,7 @@
       <c r="S18" s="1"/>
     </row>
     <row r="19" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="55" t="s">
+      <c r="A19" s="49" t="s">
         <v>67</v>
       </c>
       <c r="B19" s="46" t="s">
@@ -2398,8 +2398,8 @@
       <c r="S19" s="1"/>
     </row>
     <row r="20" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="56"/>
-      <c r="B20" s="48"/>
+      <c r="A20" s="51"/>
+      <c r="B20" s="47"/>
       <c r="C20" s="23" t="s">
         <v>73</v>
       </c>
@@ -2427,7 +2427,7 @@
       <c r="S20" s="1"/>
     </row>
     <row r="21" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="55" t="s">
+      <c r="A21" s="49" t="s">
         <v>68</v>
       </c>
       <c r="B21" s="46" t="s">
@@ -2460,8 +2460,8 @@
       <c r="S21" s="1"/>
     </row>
     <row r="22" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="56"/>
-      <c r="B22" s="48"/>
+      <c r="A22" s="51"/>
+      <c r="B22" s="47"/>
       <c r="C22" s="23" t="s">
         <v>73</v>
       </c>
@@ -2489,7 +2489,7 @@
       <c r="S22" s="1"/>
     </row>
     <row r="23" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="55" t="s">
+      <c r="A23" s="49" t="s">
         <v>69</v>
       </c>
       <c r="B23" s="46" t="s">
@@ -2522,8 +2522,8 @@
       <c r="S23" s="1"/>
     </row>
     <row r="24" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="56"/>
-      <c r="B24" s="48"/>
+      <c r="A24" s="51"/>
+      <c r="B24" s="47"/>
       <c r="C24" s="23" t="s">
         <v>73</v>
       </c>
@@ -2551,7 +2551,7 @@
       <c r="S24" s="1"/>
     </row>
     <row r="25" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="55" t="s">
+      <c r="A25" s="49" t="s">
         <v>70</v>
       </c>
       <c r="B25" s="46" t="s">
@@ -2584,8 +2584,8 @@
       <c r="S25" s="1"/>
     </row>
     <row r="26" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="56"/>
-      <c r="B26" s="48"/>
+      <c r="A26" s="51"/>
+      <c r="B26" s="47"/>
       <c r="C26" s="23" t="s">
         <v>73</v>
       </c>
@@ -2613,7 +2613,7 @@
       <c r="S26" s="1"/>
     </row>
     <row r="27" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="55" t="s">
+      <c r="A27" s="49" t="s">
         <v>71</v>
       </c>
       <c r="B27" s="57" t="s">
@@ -2646,7 +2646,7 @@
       <c r="S27" s="1"/>
     </row>
     <row r="28" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A28" s="56"/>
+      <c r="A28" s="51"/>
       <c r="B28" s="58"/>
       <c r="C28" s="22" t="s">
         <v>75</v>
@@ -2708,8 +2708,8 @@
       <c r="S29" s="1"/>
     </row>
     <row r="30" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="48"/>
-      <c r="B30" s="48"/>
+      <c r="A30" s="47"/>
+      <c r="B30" s="47"/>
       <c r="C30" s="38" t="s">
         <v>81</v>
       </c>
@@ -2770,8 +2770,8 @@
       <c r="S31" s="1"/>
     </row>
     <row r="32" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="47"/>
-      <c r="B32" s="47"/>
+      <c r="A32" s="48"/>
+      <c r="B32" s="48"/>
       <c r="C32" s="40" t="s">
         <v>83</v>
       </c>
@@ -2799,8 +2799,8 @@
       <c r="S32" s="1"/>
     </row>
     <row r="33" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="47"/>
-      <c r="B33" s="47"/>
+      <c r="A33" s="48"/>
+      <c r="B33" s="48"/>
       <c r="C33" s="41" t="s">
         <v>84</v>
       </c>
@@ -2828,8 +2828,8 @@
       <c r="S33" s="1"/>
     </row>
     <row r="34" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="47"/>
-      <c r="B34" s="47"/>
+      <c r="A34" s="48"/>
+      <c r="B34" s="48"/>
       <c r="C34" s="42" t="s">
         <v>85</v>
       </c>
@@ -2857,8 +2857,8 @@
       <c r="S34" s="1"/>
     </row>
     <row r="35" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="48"/>
-      <c r="B35" s="48"/>
+      <c r="A35" s="47"/>
+      <c r="B35" s="47"/>
       <c r="C35" s="42" t="s">
         <v>86</v>
       </c>
@@ -2919,8 +2919,8 @@
       <c r="S36" s="1"/>
     </row>
     <row r="37" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A37" s="48"/>
-      <c r="B37" s="48"/>
+      <c r="A37" s="47"/>
+      <c r="B37" s="47"/>
       <c r="C37" s="39" t="s">
         <v>88</v>
       </c>
@@ -2948,15 +2948,19 @@
       <c r="S37" s="1"/>
     </row>
     <row r="38" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="49" t="s">
+      <c r="A38" s="59" t="s">
         <v>92</v>
       </c>
       <c r="B38" s="46"/>
       <c r="C38" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="D38" s="35"/>
-      <c r="E38" s="35"/>
+      <c r="D38" s="29">
+        <v>3.2</v>
+      </c>
+      <c r="E38" s="29">
+        <v>3.2</v>
+      </c>
       <c r="F38" s="6">
         <v>6</v>
       </c>
@@ -2975,13 +2979,17 @@
       <c r="S38" s="1"/>
     </row>
     <row r="39" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="50"/>
-      <c r="B39" s="47"/>
+      <c r="A39" s="60"/>
+      <c r="B39" s="48"/>
       <c r="C39" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="D39" s="35"/>
-      <c r="E39" s="35"/>
+      <c r="D39" s="29">
+        <v>3.5</v>
+      </c>
+      <c r="E39" s="29">
+        <v>3.5</v>
+      </c>
       <c r="F39" s="6">
         <v>6</v>
       </c>
@@ -3000,13 +3008,17 @@
       <c r="S39" s="1"/>
     </row>
     <row r="40" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="51"/>
-      <c r="B40" s="48"/>
+      <c r="A40" s="61"/>
+      <c r="B40" s="47"/>
       <c r="C40" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="D40" s="35"/>
-      <c r="E40" s="35"/>
+      <c r="D40" s="29">
+        <v>4</v>
+      </c>
+      <c r="E40" s="29">
+        <v>4</v>
+      </c>
       <c r="F40" s="6">
         <v>6</v>
       </c>
@@ -3025,7 +3037,7 @@
       <c r="S40" s="1"/>
     </row>
     <row r="41" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="52" t="s">
+      <c r="A41" s="62" t="s">
         <v>93</v>
       </c>
       <c r="B41" s="46" t="s">
@@ -3034,7 +3046,7 @@
       <c r="C41" s="39" t="s">
         <v>99</v>
       </c>
-      <c r="D41" s="43">
+      <c r="D41" s="44">
         <v>3.5</v>
       </c>
       <c r="E41" s="43">
@@ -3058,8 +3070,8 @@
       <c r="S41" s="1"/>
     </row>
     <row r="42" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="53"/>
-      <c r="B42" s="47"/>
+      <c r="A42" s="63"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="39" t="s">
         <v>100</v>
       </c>
@@ -3087,8 +3099,8 @@
       <c r="S42" s="1"/>
     </row>
     <row r="43" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="53"/>
-      <c r="B43" s="47"/>
+      <c r="A43" s="63"/>
+      <c r="B43" s="48"/>
       <c r="C43" s="41" t="s">
         <v>101</v>
       </c>
@@ -3116,8 +3128,8 @@
       <c r="S43" s="1"/>
     </row>
     <row r="44" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="53"/>
-      <c r="B44" s="47"/>
+      <c r="A44" s="63"/>
+      <c r="B44" s="48"/>
       <c r="C44" s="42" t="s">
         <v>101</v>
       </c>
@@ -3145,8 +3157,8 @@
       <c r="S44" s="1"/>
     </row>
     <row r="45" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="54"/>
-      <c r="B45" s="48"/>
+      <c r="A45" s="64"/>
+      <c r="B45" s="47"/>
       <c r="C45" s="41" t="s">
         <v>112</v>
       </c>
@@ -3174,7 +3186,7 @@
       <c r="S45" s="1"/>
     </row>
     <row r="46" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="52" t="s">
+      <c r="A46" s="62" t="s">
         <v>94</v>
       </c>
       <c r="B46" s="46" t="s">
@@ -3183,8 +3195,12 @@
       <c r="C46" s="42" t="s">
         <v>102</v>
       </c>
-      <c r="D46" s="35"/>
-      <c r="E46" s="35"/>
+      <c r="D46" s="35">
+        <v>3</v>
+      </c>
+      <c r="E46" s="35">
+        <v>3</v>
+      </c>
       <c r="F46" s="6">
         <v>6</v>
       </c>
@@ -3203,13 +3219,17 @@
       <c r="S46" s="1"/>
     </row>
     <row r="47" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="54"/>
-      <c r="B47" s="48"/>
+      <c r="A47" s="64"/>
+      <c r="B47" s="47"/>
       <c r="C47" s="42" t="s">
         <v>103</v>
       </c>
-      <c r="D47" s="35"/>
-      <c r="E47" s="35"/>
+      <c r="D47" s="35">
+        <v>2.75</v>
+      </c>
+      <c r="E47" s="35">
+        <v>2.75</v>
+      </c>
       <c r="F47" s="6">
         <v>6</v>
       </c>
@@ -3228,7 +3248,7 @@
       <c r="S47" s="1"/>
     </row>
     <row r="48" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="52" t="s">
+      <c r="A48" s="62" t="s">
         <v>95</v>
       </c>
       <c r="B48" s="46" t="s">
@@ -3237,8 +3257,12 @@
       <c r="C48" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="D48" s="35"/>
-      <c r="E48" s="35"/>
+      <c r="D48" s="35">
+        <v>2</v>
+      </c>
+      <c r="E48" s="35">
+        <v>2</v>
+      </c>
       <c r="F48" s="6">
         <v>6</v>
       </c>
@@ -3257,13 +3281,17 @@
       <c r="S48" s="1"/>
     </row>
     <row r="49" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="54"/>
-      <c r="B49" s="48"/>
+      <c r="A49" s="64"/>
+      <c r="B49" s="47"/>
       <c r="C49" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="D49" s="35"/>
-      <c r="E49" s="35"/>
+      <c r="D49" s="35">
+        <v>6</v>
+      </c>
+      <c r="E49" s="35">
+        <v>6</v>
+      </c>
       <c r="F49" s="6">
         <v>6</v>
       </c>
@@ -3593,11 +3621,11 @@
       <c r="C64" s="10"/>
       <c r="D64" s="11">
         <f>SUM(D4:D63)</f>
-        <v>157.07999999999998</v>
+        <v>181.52999999999997</v>
       </c>
       <c r="E64" s="11">
         <f>SUM(E4:E57)</f>
-        <v>157.07999999999998</v>
+        <v>181.52999999999997</v>
       </c>
       <c r="F64" s="6"/>
       <c r="G64" s="1"/>
@@ -3619,17 +3647,14 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B31:B35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A31:A35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="B8:B14"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="B41:B45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="A41:A45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A48:A49"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="B19:B20"/>
@@ -3640,14 +3665,17 @@
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="B41:B45"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="A41:A45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="B8:B14"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A35"/>
+    <mergeCell ref="A36:A37"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -3662,7 +3690,7 @@
   <dimension ref="A1:X9"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3683,20 +3711,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="68"/>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68" t="s">
+      <c r="A1" s="65"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
       <c r="M1" s="12"/>
       <c r="N1" s="12"/>
       <c r="O1" s="1"/>
@@ -3711,40 +3739,40 @@
       <c r="X1" s="1"/>
     </row>
     <row r="2" spans="1:24" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="71" t="s">
+      <c r="C2" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="71" t="s">
+      <c r="D2" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="71" t="s">
+      <c r="E2" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="65" t="s">
+      <c r="F2" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="72" t="s">
+      <c r="G2" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="72" t="s">
+      <c r="H2" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="65" t="s">
+      <c r="I2" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="65" t="s">
+      <c r="J2" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="65" t="s">
+      <c r="K2" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="65" t="s">
+      <c r="L2" s="69" t="s">
         <v>23</v>
       </c>
       <c r="O2" s="1"/>
@@ -3759,18 +3787,18 @@
       <c r="X2" s="1"/>
     </row>
     <row r="3" spans="1:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="69"/>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="65"/>
+      <c r="A3" s="66"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
+      <c r="K3" s="69"/>
+      <c r="L3" s="69"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
@@ -3900,23 +3928,23 @@
       </c>
       <c r="H6" s="18">
         <f t="shared" si="1"/>
-        <v>342.91999999999996</v>
+        <v>318.46999999999997</v>
       </c>
       <c r="I6" s="18">
         <f t="shared" si="1"/>
-        <v>342.91999999999996</v>
+        <v>318.46999999999997</v>
       </c>
       <c r="J6" s="18">
         <f t="shared" si="1"/>
-        <v>342.91999999999996</v>
+        <v>318.46999999999997</v>
       </c>
       <c r="K6" s="18">
         <f t="shared" si="1"/>
-        <v>342.91999999999996</v>
+        <v>318.46999999999997</v>
       </c>
       <c r="L6" s="18">
         <f t="shared" si="1"/>
-        <v>342.91999999999996</v>
+        <v>318.46999999999997</v>
       </c>
       <c r="M6" s="19"/>
       <c r="N6" s="19"/>
@@ -3958,22 +3986,22 @@
       <c r="X7" s="1"/>
     </row>
     <row r="8" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="66" t="s">
+      <c r="A8" s="71" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="66"/>
-      <c r="C8" s="66" t="s">
+      <c r="B8" s="71"/>
+      <c r="C8" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="66"/>
-      <c r="E8" s="66"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="66"/>
-      <c r="H8" s="66"/>
-      <c r="I8" s="66"/>
-      <c r="J8" s="66"/>
-      <c r="K8" s="66"/>
-      <c r="L8" s="66"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="71"/>
+      <c r="I8" s="71"/>
+      <c r="J8" s="71"/>
+      <c r="K8" s="71"/>
+      <c r="L8" s="71"/>
       <c r="M8" s="20" t="s">
         <v>10</v>
       </c>
@@ -3992,10 +4020,10 @@
       <c r="X8" s="1"/>
     </row>
     <row r="9" spans="1:24" ht="18" x14ac:dyDescent="0.2">
-      <c r="A9" s="67">
+      <c r="A9" s="72">
         <v>50</v>
       </c>
-      <c r="B9" s="67"/>
+      <c r="B9" s="72"/>
       <c r="C9" s="18">
         <f>SUMIF('Product Backlog'!F:F,1,'Product Backlog'!E:E)</f>
         <v>39</v>
@@ -4018,7 +4046,7 @@
       </c>
       <c r="H9" s="18">
         <f>SUMIF('Product Backlog'!F:F,6,'Product Backlog'!E:E)</f>
-        <v>13.25</v>
+        <v>37.700000000000003</v>
       </c>
       <c r="I9" s="18">
         <f>SUMIF('Product Backlog'!F:F,7,'Product Backlog'!E:E)</f>
@@ -4038,11 +4066,11 @@
       </c>
       <c r="M9" s="18">
         <f>SUM(C9:L9)</f>
-        <v>157.08000000000001</v>
+        <v>181.53000000000003</v>
       </c>
       <c r="N9" s="18">
         <f>M9/10</f>
-        <v>15.708000000000002</v>
+        <v>18.153000000000002</v>
       </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -4057,6 +4085,9 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:L8"/>
+    <mergeCell ref="A9:B9"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:L1"/>
     <mergeCell ref="A2:A3"/>
@@ -4071,9 +4102,6 @@
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="L2:L3"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:L8"/>
-    <mergeCell ref="A9:B9"/>
   </mergeCells>
   <conditionalFormatting sqref="C10:N91">
     <cfRule type="expression" dxfId="2" priority="2">

</xml_diff>